<commit_message>
test: update test logs with Daytona cwd fix verification
- Test 01 now captures output files (was 0, now 1-2 files)
- Added test 02 logs for Daytona filesystem test
- Removed stale logs from other agents (codex, gemini, qwen)
</commit_message>
<xml_diff>
--- a/packages/sdk-ts/tests/test-logs/01-all-agents-parallel/claude/run2-output/dcf_model.xlsx
+++ b/packages/sdk-ts/tests/test-logs/01-all-agents-parallel/claude/run2-output/dcf_model.xlsx
@@ -17,9 +17,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="0.0%"/>
+    <numFmt numFmtId="164" formatCode="0.0000"/>
   </numFmts>
-  <fonts count="2">
+  <fonts count="5">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
@@ -29,14 +29,32 @@
     </font>
     <font>
       <b val="1"/>
+      <sz val="14"/>
+    </font>
+    <font>
+      <b val="1"/>
+    </font>
+    <font>
+      <b val="1"/>
+      <color rgb="00FFFFFF"/>
+    </font>
+    <font>
+      <b val="1"/>
+      <sz val="12"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="004472C4"/>
+        <bgColor rgb="004472C4"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -51,15 +69,19 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="3" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="4" fontId="2" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -425,7 +447,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F22"/>
+  <dimension ref="A1:F36"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -433,391 +455,468 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col width="22" customWidth="1" min="1" max="1"/>
-    <col width="12" customWidth="1" min="2" max="2"/>
-    <col width="12" customWidth="1" min="3" max="3"/>
-    <col width="12" customWidth="1" min="4" max="4"/>
-    <col width="12" customWidth="1" min="5" max="5"/>
-    <col width="12" customWidth="1" min="6" max="6"/>
+    <col width="25" customWidth="1" min="1" max="1"/>
+    <col width="15" customWidth="1" min="2" max="2"/>
+    <col width="15" customWidth="1" min="3" max="3"/>
+    <col width="15" customWidth="1" min="4" max="4"/>
+    <col width="15" customWidth="1" min="5" max="5"/>
+    <col width="15" customWidth="1" min="6" max="6"/>
+    <col width="15" customWidth="1" min="7" max="7"/>
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="1" t="inlineStr"/>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>Year 1</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>Year 2</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>Year 3</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>Year 4</t>
-        </is>
-      </c>
-      <c r="F1" s="1" t="inlineStr">
-        <is>
-          <t>Year 5</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>Revenue</t>
-        </is>
-      </c>
-      <c r="B2" s="2" t="n">
-        <v>1000000</v>
-      </c>
-      <c r="C2" s="2" t="n">
-        <v>1100000</v>
-      </c>
-      <c r="D2" s="2" t="n">
-        <v>1210000</v>
-      </c>
-      <c r="E2" s="2" t="n">
-        <v>1331000</v>
-      </c>
-      <c r="F2" s="2" t="n">
-        <v>1464100</v>
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>5-Year DCF Model</t>
+        </is>
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>Growth Rate</t>
-        </is>
-      </c>
-      <c r="B3" s="3" t="n"/>
-      <c r="C3" s="3" t="n">
-        <v>0.1</v>
-      </c>
-      <c r="D3" s="3" t="n">
-        <v>0.1</v>
-      </c>
-      <c r="E3" s="3" t="n">
-        <v>0.1</v>
-      </c>
-      <c r="F3" s="3" t="n">
-        <v>0.1</v>
+      <c r="A3" s="2" t="inlineStr">
+        <is>
+          <t>Assumptions</t>
+        </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>EBITDA Margin</t>
+          <t>Initial Revenue</t>
         </is>
       </c>
       <c r="B4" s="3" t="n">
-        <v>0.2</v>
-      </c>
-      <c r="C4" s="3" t="n">
-        <v>0.21</v>
-      </c>
-      <c r="D4" s="3" t="n">
-        <v>0.22</v>
-      </c>
-      <c r="E4" s="3" t="n">
-        <v>0.23</v>
-      </c>
-      <c r="F4" s="3" t="n">
-        <v>0.24</v>
+        <v>1000000</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>EBITDA</t>
-        </is>
-      </c>
-      <c r="B5" s="2" t="n">
-        <v>200000</v>
-      </c>
-      <c r="C5" s="2" t="n">
-        <v>231000</v>
-      </c>
-      <c r="D5" s="2" t="n">
-        <v>266200</v>
-      </c>
-      <c r="E5" s="2" t="n">
-        <v>306130</v>
-      </c>
-      <c r="F5" s="2" t="n">
-        <v>351384</v>
+          <t>Revenue Growth Rate</t>
+        </is>
+      </c>
+      <c r="B5" s="4" t="n">
+        <v>0.1</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>D&amp;A</t>
-        </is>
-      </c>
-      <c r="B6" s="2" t="n">
-        <v>50000</v>
-      </c>
-      <c r="C6" s="2" t="n">
-        <v>55000</v>
-      </c>
-      <c r="D6" s="2" t="n">
-        <v>60500</v>
-      </c>
-      <c r="E6" s="2" t="n">
-        <v>66550</v>
-      </c>
-      <c r="F6" s="2" t="n">
-        <v>73205</v>
+          <t>EBITDA Margin</t>
+        </is>
+      </c>
+      <c r="B6" s="4" t="n">
+        <v>0.2</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>EBIT</t>
-        </is>
-      </c>
-      <c r="B7" s="2" t="n">
-        <v>150000</v>
-      </c>
-      <c r="C7" s="2" t="n">
-        <v>176000</v>
-      </c>
-      <c r="D7" s="2" t="n">
-        <v>205700</v>
-      </c>
-      <c r="E7" s="2" t="n">
-        <v>239580</v>
-      </c>
-      <c r="F7" s="2" t="n">
-        <v>278179</v>
+          <t>Tax Rate</t>
+        </is>
+      </c>
+      <c r="B7" s="4" t="n">
+        <v>0.25</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Tax Rate</t>
-        </is>
-      </c>
-      <c r="B8" s="3" t="n">
-        <v>0.25</v>
-      </c>
-      <c r="C8" s="3" t="n">
-        <v>0.25</v>
-      </c>
-      <c r="D8" s="3" t="n">
-        <v>0.25</v>
-      </c>
-      <c r="E8" s="3" t="n">
-        <v>0.25</v>
-      </c>
-      <c r="F8" s="3" t="n">
-        <v>0.25</v>
+          <t>Capex (% of Revenue)</t>
+        </is>
+      </c>
+      <c r="B8" s="4" t="n">
+        <v>0.05</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Taxes</t>
-        </is>
-      </c>
-      <c r="B9" s="2" t="n">
-        <v>37500</v>
-      </c>
-      <c r="C9" s="2" t="n">
-        <v>44000</v>
-      </c>
-      <c r="D9" s="2" t="n">
-        <v>51425</v>
-      </c>
-      <c r="E9" s="2" t="n">
-        <v>59895</v>
-      </c>
-      <c r="F9" s="2" t="n">
-        <v>69545</v>
+          <t>D&amp;A (% of Revenue)</t>
+        </is>
+      </c>
+      <c r="B9" s="4" t="n">
+        <v>0.03</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>NOPAT</t>
-        </is>
-      </c>
-      <c r="B10" s="2" t="n">
-        <v>112500</v>
-      </c>
-      <c r="C10" s="2" t="n">
-        <v>132000</v>
-      </c>
-      <c r="D10" s="2" t="n">
-        <v>154275</v>
-      </c>
-      <c r="E10" s="2" t="n">
-        <v>179685</v>
-      </c>
-      <c r="F10" s="2" t="n">
-        <v>208634</v>
+          <t>Change in NWC (% of Revenue)</t>
+        </is>
+      </c>
+      <c r="B10" s="4" t="n">
+        <v>0.02</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Add: D&amp;A</t>
-        </is>
-      </c>
-      <c r="B11" s="2" t="n">
-        <v>50000</v>
-      </c>
-      <c r="C11" s="2" t="n">
-        <v>55000</v>
-      </c>
-      <c r="D11" s="2" t="n">
-        <v>60500</v>
-      </c>
-      <c r="E11" s="2" t="n">
-        <v>66550</v>
-      </c>
-      <c r="F11" s="2" t="n">
-        <v>73205</v>
+          <t>Discount Rate (WACC)</t>
+        </is>
+      </c>
+      <c r="B11" s="4" t="n">
+        <v>0.1</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Less: CapEx</t>
-        </is>
-      </c>
-      <c r="B12" s="2" t="n">
-        <v>-60000</v>
-      </c>
-      <c r="C12" s="2" t="n">
-        <v>-66000</v>
-      </c>
-      <c r="D12" s="2" t="n">
-        <v>-72600</v>
-      </c>
-      <c r="E12" s="2" t="n">
-        <v>-79860</v>
-      </c>
-      <c r="F12" s="2" t="n">
-        <v>-87846</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="inlineStr">
-        <is>
-          <t>Less: Change in NWC</t>
-        </is>
-      </c>
-      <c r="B13" s="2" t="n">
-        <v>-10000</v>
-      </c>
-      <c r="C13" s="2" t="n">
-        <v>-10000</v>
-      </c>
-      <c r="D13" s="2" t="n">
-        <v>-11000</v>
-      </c>
-      <c r="E13" s="2" t="n">
-        <v>-12100</v>
-      </c>
-      <c r="F13" s="2" t="n">
-        <v>-13310</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="inlineStr">
-        <is>
-          <t>Free Cash Flow</t>
-        </is>
-      </c>
-      <c r="B14" s="2" t="n">
-        <v>92500</v>
-      </c>
-      <c r="C14" s="2" t="n">
-        <v>111000</v>
-      </c>
-      <c r="D14" s="2" t="n">
-        <v>131175</v>
-      </c>
-      <c r="E14" s="2" t="n">
-        <v>154275</v>
-      </c>
-      <c r="F14" s="2" t="n">
-        <v>180683</v>
+          <t>Terminal Growth Rate</t>
+        </is>
+      </c>
+      <c r="B12" s="4" t="n">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="5" t="inlineStr">
+        <is>
+          <t>Year</t>
+        </is>
+      </c>
+      <c r="B15" s="6" t="inlineStr">
+        <is>
+          <t>Year 1</t>
+        </is>
+      </c>
+      <c r="C15" s="6" t="inlineStr">
+        <is>
+          <t>Year 2</t>
+        </is>
+      </c>
+      <c r="D15" s="6" t="inlineStr">
+        <is>
+          <t>Year 3</t>
+        </is>
+      </c>
+      <c r="E15" s="6" t="inlineStr">
+        <is>
+          <t>Year 4</t>
+        </is>
+      </c>
+      <c r="F15" s="6" t="inlineStr">
+        <is>
+          <t>Year 5</t>
+        </is>
       </c>
     </row>
     <row r="16">
-      <c r="A16" s="4" t="inlineStr">
-        <is>
-          <t>DCF Valuation</t>
-        </is>
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>Revenue</t>
+        </is>
+      </c>
+      <c r="B16" s="3" t="n">
+        <v>1100000</v>
+      </c>
+      <c r="C16" s="3" t="n">
+        <v>1210000</v>
+      </c>
+      <c r="D16" s="3" t="n">
+        <v>1331000</v>
+      </c>
+      <c r="E16" s="3" t="n">
+        <v>1464100</v>
+      </c>
+      <c r="F16" s="3" t="n">
+        <v>1610510</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>Discount Rate (WACC)</t>
+          <t>EBITDA</t>
         </is>
       </c>
       <c r="B17" s="3" t="n">
-        <v>0.1</v>
+        <v>220000</v>
+      </c>
+      <c r="C17" s="3" t="n">
+        <v>242000.0000000001</v>
+      </c>
+      <c r="D17" s="3" t="n">
+        <v>266200.0000000001</v>
+      </c>
+      <c r="E17" s="3" t="n">
+        <v>292820.0000000001</v>
+      </c>
+      <c r="F17" s="3" t="n">
+        <v>322102.0000000001</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>Terminal Growth Rate</t>
+          <t>Less: D&amp;A</t>
         </is>
       </c>
       <c r="B18" s="3" t="n">
-        <v>0.02</v>
+        <v>33000</v>
+      </c>
+      <c r="C18" s="3" t="n">
+        <v>36300.00000000001</v>
+      </c>
+      <c r="D18" s="3" t="n">
+        <v>39930.00000000001</v>
+      </c>
+      <c r="E18" s="3" t="n">
+        <v>43923.00000000001</v>
+      </c>
+      <c r="F18" s="3" t="n">
+        <v>48315.30000000001</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>Terminal Value</t>
-        </is>
-      </c>
-      <c r="B19" s="2" t="n">
-        <v>2303708.25</v>
+          <t>EBIT</t>
+        </is>
+      </c>
+      <c r="B19" s="3" t="n">
+        <v>187000</v>
+      </c>
+      <c r="C19" s="3" t="n">
+        <v>205700.0000000001</v>
+      </c>
+      <c r="D19" s="3" t="n">
+        <v>226270.0000000001</v>
+      </c>
+      <c r="E19" s="3" t="n">
+        <v>248897.0000000001</v>
+      </c>
+      <c r="F19" s="3" t="n">
+        <v>273786.7000000001</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>PV of FCFs</t>
-        </is>
-      </c>
-      <c r="B20" s="2" t="n">
-        <v>491941.9935299997</v>
+          <t>Less: Taxes</t>
+        </is>
+      </c>
+      <c r="B20" s="3" t="n">
+        <v>46750</v>
+      </c>
+      <c r="C20" s="3" t="n">
+        <v>51425.00000000001</v>
+      </c>
+      <c r="D20" s="3" t="n">
+        <v>56567.50000000003</v>
+      </c>
+      <c r="E20" s="3" t="n">
+        <v>62224.25000000003</v>
+      </c>
+      <c r="F20" s="3" t="n">
+        <v>68446.67500000003</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
+          <t>EBIAT (NOPAT)</t>
+        </is>
+      </c>
+      <c r="B21" s="3" t="n">
+        <v>140250</v>
+      </c>
+      <c r="C21" s="3" t="n">
+        <v>154275.0000000001</v>
+      </c>
+      <c r="D21" s="3" t="n">
+        <v>169702.5000000001</v>
+      </c>
+      <c r="E21" s="3" t="n">
+        <v>186672.7500000001</v>
+      </c>
+      <c r="F21" s="3" t="n">
+        <v>205340.0250000001</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>Plus: D&amp;A</t>
+        </is>
+      </c>
+      <c r="B22" s="3" t="n">
+        <v>33000</v>
+      </c>
+      <c r="C22" s="3" t="n">
+        <v>36300.00000000001</v>
+      </c>
+      <c r="D22" s="3" t="n">
+        <v>39930.00000000001</v>
+      </c>
+      <c r="E22" s="3" t="n">
+        <v>43923.00000000001</v>
+      </c>
+      <c r="F22" s="3" t="n">
+        <v>48315.30000000001</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>Less: Capex</t>
+        </is>
+      </c>
+      <c r="B23" s="3" t="n">
+        <v>55000</v>
+      </c>
+      <c r="C23" s="3" t="n">
+        <v>60500.00000000001</v>
+      </c>
+      <c r="D23" s="3" t="n">
+        <v>66550.00000000003</v>
+      </c>
+      <c r="E23" s="3" t="n">
+        <v>73205.00000000003</v>
+      </c>
+      <c r="F23" s="3" t="n">
+        <v>80525.50000000003</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>Less: Change in NWC</t>
+        </is>
+      </c>
+      <c r="B24" s="3" t="n">
+        <v>22000</v>
+      </c>
+      <c r="C24" s="3" t="n">
+        <v>24200</v>
+      </c>
+      <c r="D24" s="3" t="n">
+        <v>26620.00000000001</v>
+      </c>
+      <c r="E24" s="3" t="n">
+        <v>29282.00000000001</v>
+      </c>
+      <c r="F24" s="3" t="n">
+        <v>32210.20000000001</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>Free Cash Flow</t>
+        </is>
+      </c>
+      <c r="B25" s="3" t="n">
+        <v>96250</v>
+      </c>
+      <c r="C25" s="3" t="n">
+        <v>105875</v>
+      </c>
+      <c r="D25" s="3" t="n">
+        <v>116462.5000000001</v>
+      </c>
+      <c r="E25" s="3" t="n">
+        <v>128108.7500000001</v>
+      </c>
+      <c r="F25" s="3" t="n">
+        <v>140919.6250000001</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr"/>
+      <c r="B26" t="inlineStr"/>
+      <c r="C26" t="inlineStr"/>
+      <c r="D26" t="inlineStr"/>
+      <c r="E26" t="inlineStr"/>
+      <c r="F26" t="inlineStr"/>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>Discount Factor</t>
+        </is>
+      </c>
+      <c r="B27" s="7" t="n">
+        <v>0.9090909090909091</v>
+      </c>
+      <c r="C27" s="7" t="n">
+        <v>0.8264462809917354</v>
+      </c>
+      <c r="D27" s="7" t="n">
+        <v>0.7513148009015775</v>
+      </c>
+      <c r="E27" s="7" t="n">
+        <v>0.6830134553650705</v>
+      </c>
+      <c r="F27" s="7" t="n">
+        <v>0.6209213230591549</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>Present Value of FCF</t>
+        </is>
+      </c>
+      <c r="B28" s="3" t="n">
+        <v>87500</v>
+      </c>
+      <c r="C28" s="3" t="n">
+        <v>87500.00000000003</v>
+      </c>
+      <c r="D28" s="3" t="n">
+        <v>87500.00000000003</v>
+      </c>
+      <c r="E28" s="3" t="n">
+        <v>87500.00000000003</v>
+      </c>
+      <c r="F28" s="3" t="n">
+        <v>87500</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" s="8" t="inlineStr">
+        <is>
+          <t>Valuation Summary</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>Sum of PV of FCFs</t>
+        </is>
+      </c>
+      <c r="B33" s="3" t="n">
+        <v>437500.0000000001</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>Terminal Value</t>
+        </is>
+      </c>
+      <c r="B34" s="3" t="n">
+        <v>1796725.218750001</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
           <t>PV of Terminal Value</t>
         </is>
       </c>
-      <c r="B21" s="2" t="n">
-        <v>1430421.57453229</v>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" s="4" t="inlineStr">
+      <c r="B35" s="3" t="n">
+        <v>1115625</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" s="2" t="inlineStr">
         <is>
           <t>Enterprise Value</t>
         </is>
       </c>
-      <c r="B22" s="5" t="n">
-        <v>1922363.56806229</v>
+      <c r="B36" s="9" t="n">
+        <v>1553125</v>
       </c>
     </row>
   </sheetData>

</xml_diff>